<commit_message>
HiTechnic and Mindsensors Compass, Acceleration and Gyro sensors
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="121">
   <si>
     <t>AccelHTSensor</t>
   </si>
@@ -337,16 +337,69 @@
   </si>
   <si>
     <t>Lawrie</t>
+  </si>
+  <si>
+    <t>Acceleration</t>
+  </si>
+  <si>
+    <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NAC1040</t>
+  </si>
+  <si>
+    <t>Tilt</t>
+  </si>
+  <si>
+    <t>Compass</t>
+  </si>
+  <si>
+    <t>HiTechnicAccelerometer</t>
+  </si>
+  <si>
+    <t>MindsensorsCompass</t>
+  </si>
+  <si>
+    <t>http://www.mindsensors.com/index.php?module=pagemaster&amp;PAGE_user_op=view_page&amp;PAGE_id=101</t>
+  </si>
+  <si>
+    <t>Gyro</t>
+  </si>
+  <si>
+    <t>HiTechnicGyro</t>
+  </si>
+  <si>
+    <t>MindsensorsAccelerometer</t>
+  </si>
+  <si>
+    <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NMC1034</t>
+  </si>
+  <si>
+    <t>HiTechnicCompass</t>
+  </si>
+  <si>
+    <t>http://www.mindsensors.com/index.php?module=pagemaster&amp;PAGE_user_op=view_page&amp;PAGE_id=56</t>
+  </si>
+  <si>
+    <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NGY1044</t>
+  </si>
+  <si>
+    <t>CalibratedSampleProvider</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -369,13 +422,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -678,20 +734,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
     <col min="9" max="9" width="53" customWidth="1"/>
   </cols>
@@ -729,40 +788,67 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
       <c r="C2" t="s">
         <v>84</v>
       </c>
       <c r="D2" t="s">
         <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
       <c r="C3" t="s">
         <v>84</v>
       </c>
       <c r="D3" t="s">
         <v>105</v>
       </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="F4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>84</v>
@@ -770,34 +856,34 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>84</v>
@@ -805,18 +891,48 @@
       <c r="D10" t="s">
         <v>105</v>
       </c>
+      <c r="E10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" t="s">
+        <v>120</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
       </c>
       <c r="C11" t="s">
         <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
@@ -824,7 +940,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
         <v>84</v>
@@ -832,15 +948,15 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
         <v>90</v>
@@ -848,15 +964,15 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
         <v>84</v>
@@ -864,7 +980,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
         <v>84</v>
@@ -872,7 +988,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
         <v>84</v>
@@ -880,150 +996,165 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
         <v>85</v>
       </c>
-      <c r="E21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" t="s">
-        <v>89</v>
+      <c r="E22" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>23</v>
       </c>
-      <c r="C26" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
         <v>85</v>
       </c>
-      <c r="E26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" t="s">
         <v>86</v>
-      </c>
-      <c r="G26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
-        <v>88</v>
       </c>
       <c r="G27" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" t="s">
-        <v>84</v>
-      </c>
-      <c r="H28" t="s">
-        <v>92</v>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
-      </c>
-      <c r="I29" t="s">
-        <v>93</v>
+        <v>84</v>
+      </c>
+      <c r="H29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="I30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>114</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I31" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C32" t="s">
         <v>90</v>
-      </c>
-      <c r="H32" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>90</v>
+      </c>
+      <c r="H33" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
         <v>96</v>
@@ -1031,56 +1162,56 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>104</v>
       </c>
       <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
         <v>90</v>
@@ -1088,7 +1219,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C41" t="s">
         <v>90</v>
@@ -1096,7 +1227,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" t="s">
         <v>90</v>
@@ -1104,34 +1235,34 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
-      </c>
-      <c r="H43" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
         <v>84</v>
+      </c>
+      <c r="H44" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
         <v>90</v>
@@ -1139,7 +1270,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
         <v>90</v>
@@ -1147,7 +1278,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
         <v>90</v>
@@ -1155,7 +1286,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" t="s">
         <v>90</v>
@@ -1163,83 +1294,83 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
         <v>90</v>
-      </c>
-      <c r="H50" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
         <v>90</v>
+      </c>
+      <c r="H51" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>84</v>
-      </c>
-      <c r="H54" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
         <v>90</v>
       </c>
       <c r="H56" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57" t="s">
         <v>90</v>
+      </c>
+      <c r="H57" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58" t="s">
         <v>90</v>
@@ -1247,7 +1378,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
         <v>90</v>
@@ -1255,84 +1386,84 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>65</v>
-      </c>
-      <c r="C69" t="s">
-        <v>90</v>
-      </c>
-      <c r="H69" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70" t="s">
         <v>90</v>
+      </c>
+      <c r="H70" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="C71" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
         <v>90</v>
@@ -1340,71 +1471,83 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>84</v>
-      </c>
-      <c r="D74" t="s">
-        <v>85</v>
-      </c>
-      <c r="E74" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="B75" t="s">
+        <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>96</v>
+        <v>84</v>
+      </c>
+      <c r="D75" t="s">
+        <v>85</v>
+      </c>
+      <c r="E75" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>74</v>
+      </c>
+      <c r="C79" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>75</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>102</v>
       </c>
-      <c r="C79" t="s">
-        <v>84</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="C80" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" t="s">
         <v>85</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E80" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H10" r:id="rId1"/>
+    <hyperlink ref="H31" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Claimed 3 more sensors
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
   <si>
     <t>AccelHTSensor</t>
   </si>
@@ -382,6 +382,21 @@
   </si>
   <si>
     <t>CalibratedSampleProvider</t>
+  </si>
+  <si>
+    <t>HiTechnicEOPD</t>
+  </si>
+  <si>
+    <t>DexterPressureSensor250</t>
+  </si>
+  <si>
+    <t>DexterPressureSensor500</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
@@ -740,7 +755,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,16 +989,46 @@
       <c r="A17" t="s">
         <v>14</v>
       </c>
+      <c r="B17" t="s">
+        <v>122</v>
+      </c>
       <c r="C17" t="s">
         <v>84</v>
+      </c>
+      <c r="D17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
+      <c r="B18" t="s">
+        <v>123</v>
+      </c>
       <c r="C18" t="s">
         <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -998,8 +1043,23 @@
       <c r="A20" t="s">
         <v>17</v>
       </c>
+      <c r="B20" t="s">
+        <v>121</v>
+      </c>
       <c r="C20" t="s">
         <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Two Dexter pressure sensors and a HiTechnic EOPD
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="128">
   <si>
     <t>AccelHTSensor</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>Distance</t>
+  </si>
+  <si>
+    <t>http://www.dexterindustries.com/Products-dPressure.html</t>
+  </si>
+  <si>
+    <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NEO1048</t>
   </si>
 </sst>
 </file>
@@ -752,10 +758,10 @@
   <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,6 +1013,9 @@
       <c r="G17" t="s">
         <v>87</v>
       </c>
+      <c r="H17" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1030,6 +1039,9 @@
       <c r="G18" t="s">
         <v>87</v>
       </c>
+      <c r="H18" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1061,6 +1073,9 @@
       <c r="G20" t="s">
         <v>87</v>
       </c>
+      <c r="H20" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1456,6 +1471,9 @@
       <c r="A61" t="s">
         <v>56</v>
       </c>
+      <c r="C61" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
@@ -1495,6 +1513,9 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>64</v>
+      </c>
+      <c r="C69" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Claimed two more sensors
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
   <si>
     <t>AccelHTSensor</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NEO1048</t>
+  </si>
+  <si>
+    <t>Temperature</t>
   </si>
 </sst>
 </file>
@@ -758,10 +761,10 @@
   <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C57" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C69" sqref="C69"/>
+      <selection pane="bottomRight" activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,6 +1337,18 @@
       <c r="C45" t="s">
         <v>84</v>
       </c>
+      <c r="D45" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" t="s">
+        <v>90</v>
+      </c>
+      <c r="F45" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1516,6 +1531,18 @@
       </c>
       <c r="C69" t="s">
         <v>84</v>
+      </c>
+      <c r="D69" t="s">
+        <v>105</v>
+      </c>
+      <c r="E69" t="s">
+        <v>90</v>
+      </c>
+      <c r="F69" t="s">
+        <v>128</v>
+      </c>
+      <c r="G69" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Mindsensors pressure sensor and RCX thermometer
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="132">
   <si>
     <t>AccelHTSensor</t>
   </si>
@@ -406,6 +406,15 @@
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>http://www.mindsensors.com/index.php?module=pagemaster&amp;PAGE_user_op=view_page&amp;PAGE_id=150</t>
+  </si>
+  <si>
+    <t>MindsensorsPressureSensor</t>
+  </si>
+  <si>
+    <t>RCXThermometer</t>
   </si>
 </sst>
 </file>
@@ -764,7 +773,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I66" sqref="I66"/>
+      <selection pane="bottomRight" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,6 +1343,9 @@
       <c r="A45" t="s">
         <v>40</v>
       </c>
+      <c r="B45" t="s">
+        <v>130</v>
+      </c>
       <c r="C45" t="s">
         <v>84</v>
       </c>
@@ -1348,6 +1360,9 @@
       </c>
       <c r="G45" t="s">
         <v>87</v>
+      </c>
+      <c r="H45" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1528,6 +1543,9 @@
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>64</v>
+      </c>
+      <c r="B69" t="s">
+        <v>131</v>
       </c>
       <c r="C69" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Claimed another two sensors
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="135">
   <si>
     <t>AccelHTSensor</t>
   </si>
@@ -415,6 +415,15 @@
   </si>
   <si>
     <t>RCXThermometer</t>
+  </si>
+  <si>
+    <t>Magnetic</t>
+  </si>
+  <si>
+    <t>HiTechnicMagneticSensor</t>
+  </si>
+  <si>
+    <t>Light</t>
   </si>
 </sst>
 </file>
@@ -773,7 +782,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B69" sqref="B69"/>
+      <selection pane="bottomRight" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,8 +1341,23 @@
       <c r="A44" t="s">
         <v>39</v>
       </c>
+      <c r="B44" t="s">
+        <v>133</v>
+      </c>
       <c r="C44" t="s">
         <v>84</v>
+      </c>
+      <c r="D44" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" t="s">
+        <v>132</v>
+      </c>
+      <c r="G44" t="s">
+        <v>87</v>
       </c>
       <c r="H44" t="s">
         <v>97</v>
@@ -1501,43 +1525,79 @@
       <c r="A61" t="s">
         <v>56</v>
       </c>
+      <c r="B61" t="s">
+        <v>56</v>
+      </c>
       <c r="C61" t="s">
         <v>84</v>
+      </c>
+      <c r="D61" t="s">
+        <v>105</v>
+      </c>
+      <c r="E61" t="s">
+        <v>90</v>
+      </c>
+      <c r="F61" t="s">
+        <v>134</v>
+      </c>
+      <c r="G61" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>57</v>
       </c>
+      <c r="C62" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>58</v>
       </c>
+      <c r="C63" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>59</v>
       </c>
+      <c r="C64" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>60</v>
       </c>
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>61</v>
       </c>
+      <c r="C66" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>62</v>
       </c>
+      <c r="C67" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Converted HiTechnic Magnetic sensor
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -312,9 +312,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>hitechnic</t>
-  </si>
-  <si>
     <t>mindsensors</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>Light</t>
+  </si>
+  <si>
+    <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NMS1035</t>
   </si>
 </sst>
 </file>
@@ -782,7 +782,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C68" sqref="C68"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,25 +831,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
         <v>84</v>
       </c>
       <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
         <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" t="s">
-        <v>106</v>
       </c>
       <c r="G2" t="s">
         <v>87</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -857,30 +857,30 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
         <v>84</v>
       </c>
       <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" t="s">
         <v>105</v>
-      </c>
-      <c r="E3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" t="s">
-        <v>106</v>
       </c>
       <c r="G3" t="s">
         <v>87</v>
       </c>
       <c r="H3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -925,25 +925,25 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
         <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" t="s">
         <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -951,25 +951,25 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
         <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
         <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1017,25 +1017,25 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
         <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E17" t="s">
         <v>90</v>
       </c>
       <c r="F17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G17" t="s">
         <v>87</v>
       </c>
       <c r="H17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1043,25 +1043,25 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" t="s">
         <v>123</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" t="s">
-        <v>124</v>
       </c>
       <c r="G18" t="s">
         <v>87</v>
       </c>
       <c r="H18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1077,25 +1077,25 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
         <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E20" t="s">
         <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G20" t="s">
         <v>87</v>
       </c>
       <c r="H20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,25 +1205,25 @@
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C31" t="s">
         <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E31" t="s">
         <v>90</v>
       </c>
       <c r="F31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G31" t="s">
         <v>87</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I31" t="s">
         <v>94</v>
@@ -1293,7 +1293,7 @@
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
         <v>84</v>
@@ -1342,25 +1342,25 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
         <v>84</v>
       </c>
       <c r="D44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E44" t="s">
         <v>90</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G44" t="s">
         <v>87</v>
       </c>
       <c r="H44" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1368,25 +1368,25 @@
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C45" t="s">
         <v>84</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E45" t="s">
         <v>90</v>
       </c>
       <c r="F45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G45" t="s">
         <v>87</v>
       </c>
       <c r="H45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
         <v>90</v>
       </c>
       <c r="H51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
         <v>84</v>
       </c>
       <c r="H55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,7 +1483,7 @@
         <v>90</v>
       </c>
       <c r="H56" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>90</v>
       </c>
       <c r="H57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1532,13 +1532,13 @@
         <v>84</v>
       </c>
       <c r="D61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E61" t="s">
         <v>90</v>
       </c>
       <c r="F61" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G61" t="s">
         <v>87</v>
@@ -1605,19 +1605,19 @@
         <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C69" t="s">
         <v>84</v>
       </c>
       <c r="D69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E69" t="s">
         <v>90</v>
       </c>
       <c r="F69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G69" t="s">
         <v>87</v>
@@ -1631,7 +1631,7 @@
         <v>90</v>
       </c>
       <c r="H70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
         <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C75" t="s">
         <v>84</v>
@@ -1717,7 +1717,7 @@
         <v>75</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C80" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Claimed the two IRSeeker classes
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="142">
   <si>
     <t>AccelHTSensor</t>
   </si>
@@ -430,6 +430,21 @@
   </si>
   <si>
     <t>SamplerProvider</t>
+  </si>
+  <si>
+    <t>Angular Velocity</t>
+  </si>
+  <si>
+    <t>Accumulated Angle</t>
+  </si>
+  <si>
+    <t>HiTechnicAngleSensor</t>
+  </si>
+  <si>
+    <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NAA1030</t>
+  </si>
+  <si>
+    <t>HiTechnicBarometer</t>
   </si>
 </sst>
 </file>
@@ -782,13 +797,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +812,7 @@
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.140625" customWidth="1"/>
     <col min="8" max="8" width="27" customWidth="1"/>
     <col min="9" max="9" width="53" customWidth="1"/>
@@ -888,6 +903,9 @@
       <c r="F4" t="s">
         <v>107</v>
       </c>
+      <c r="G4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -898,6 +916,9 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
       <c r="C6" t="s">
         <v>84</v>
       </c>
@@ -913,98 +934,68 @@
       <c r="G6" t="s">
         <v>136</v>
       </c>
+      <c r="H6" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
-      </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="G7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
+      <c r="F8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
       </c>
       <c r="C9" t="s">
         <v>84</v>
       </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" t="s">
-        <v>90</v>
-      </c>
       <c r="F10" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G11" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
@@ -1012,102 +1003,102 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>116</v>
       </c>
       <c r="C13" t="s">
         <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>110</v>
       </c>
       <c r="C14" t="s">
         <v>84</v>
+      </c>
+      <c r="D14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>120</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" t="s">
-        <v>122</v>
-      </c>
-      <c r="G17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" t="s">
-        <v>122</v>
-      </c>
-      <c r="G18" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>119</v>
       </c>
       <c r="C20" t="s">
         <v>84</v>
@@ -1119,333 +1110,387 @@
         <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G20" t="s">
         <v>87</v>
       </c>
       <c r="H20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>20</v>
       </c>
       <c r="C24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" t="s">
         <v>85</v>
       </c>
-      <c r="E27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" t="s">
         <v>86</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G30" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>88</v>
-      </c>
-      <c r="G28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
-      <c r="H29" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" t="s">
-        <v>90</v>
-      </c>
-      <c r="I30" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" t="s">
-        <v>90</v>
-      </c>
-      <c r="F31" t="s">
-        <v>112</v>
       </c>
       <c r="G31" t="s">
         <v>87</v>
       </c>
-      <c r="H31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="H32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>90</v>
+      </c>
+      <c r="I33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s">
+        <v>104</v>
+      </c>
+      <c r="E34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F34" t="s">
+        <v>112</v>
+      </c>
+      <c r="G34" t="s">
+        <v>87</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I34" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>27</v>
       </c>
-      <c r="C32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>28</v>
       </c>
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>29</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" t="s">
+        <v>90</v>
+      </c>
+      <c r="G37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>30</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C38" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>31</v>
       </c>
-      <c r="C36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>32</v>
       </c>
-      <c r="C37" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>33</v>
       </c>
-      <c r="C38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="C41" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>34</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>103</v>
       </c>
-      <c r="C39" t="s">
-        <v>84</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C42" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" t="s">
         <v>85</v>
       </c>
-      <c r="E39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="E42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>35</v>
       </c>
-      <c r="C40" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>36</v>
       </c>
-      <c r="C41" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>37</v>
       </c>
-      <c r="C42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>38</v>
       </c>
-      <c r="C43" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>39</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>131</v>
       </c>
-      <c r="C44" t="s">
-        <v>84</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="C47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" t="s">
         <v>104</v>
       </c>
-      <c r="E44" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="E47" t="s">
+        <v>90</v>
+      </c>
+      <c r="F47" t="s">
         <v>130</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G47" t="s">
         <v>87</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H47" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>40</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B48" t="s">
         <v>128</v>
       </c>
-      <c r="C45" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C48" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" t="s">
         <v>104</v>
       </c>
-      <c r="E45" t="s">
-        <v>90</v>
-      </c>
-      <c r="F45" t="s">
+      <c r="E48" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" t="s">
         <v>122</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G48" t="s">
         <v>87</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H48" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C49" t="s">
         <v>90</v>
@@ -1453,7 +1498,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C50" t="s">
         <v>90</v>
@@ -1461,18 +1506,15 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C51" t="s">
         <v>90</v>
-      </c>
-      <c r="H51" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
         <v>90</v>
@@ -1480,103 +1522,91 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C54" t="s">
         <v>90</v>
+      </c>
+      <c r="H54" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C55" t="s">
-        <v>84</v>
-      </c>
-      <c r="H55" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>90</v>
-      </c>
-      <c r="H56" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C57" t="s">
         <v>90</v>
-      </c>
-      <c r="H57" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C58" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="H58" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C59" t="s">
         <v>90</v>
+      </c>
+      <c r="H59" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C60" t="s">
         <v>90</v>
+      </c>
+      <c r="H60" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C61" t="s">
-        <v>84</v>
-      </c>
-      <c r="D61" t="s">
-        <v>104</v>
-      </c>
-      <c r="E61" t="s">
-        <v>90</v>
-      </c>
-      <c r="F61" t="s">
-        <v>132</v>
-      </c>
-      <c r="G61" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
         <v>90</v>
@@ -1584,7 +1614,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
         <v>90</v>
@@ -1592,15 +1622,30 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="B64" t="s">
+        <v>56</v>
       </c>
       <c r="C64" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="D64" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" t="s">
+        <v>90</v>
+      </c>
+      <c r="F64" t="s">
+        <v>132</v>
+      </c>
+      <c r="G64" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
         <v>90</v>
@@ -1608,7 +1653,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C66" t="s">
         <v>90</v>
@@ -1616,15 +1661,15 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C67" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C68" t="s">
         <v>90</v>
@@ -1632,41 +1677,23 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>64</v>
-      </c>
-      <c r="B69" t="s">
-        <v>129</v>
+        <v>61</v>
       </c>
       <c r="C69" t="s">
-        <v>84</v>
-      </c>
-      <c r="D69" t="s">
-        <v>104</v>
-      </c>
-      <c r="E69" t="s">
-        <v>90</v>
-      </c>
-      <c r="F69" t="s">
-        <v>126</v>
-      </c>
-      <c r="G69" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>90</v>
-      </c>
-      <c r="H70" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C71" t="s">
         <v>90</v>
@@ -1674,20 +1701,41 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>64</v>
+      </c>
+      <c r="B72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72" t="s">
+        <v>104</v>
+      </c>
+      <c r="E72" t="s">
+        <v>90</v>
+      </c>
+      <c r="F72" t="s">
+        <v>126</v>
+      </c>
+      <c r="G72" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C73" t="s">
         <v>90</v>
+      </c>
+      <c r="H73" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C74" t="s">
         <v>90</v>
@@ -1695,32 +1743,20 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" t="s">
-        <v>102</v>
-      </c>
-      <c r="C75" t="s">
-        <v>84</v>
-      </c>
-      <c r="D75" t="s">
-        <v>85</v>
-      </c>
-      <c r="E75" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C76" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C77" t="s">
         <v>90</v>
@@ -1728,41 +1764,74 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="B78" t="s">
+        <v>102</v>
       </c>
       <c r="C78" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="D78" t="s">
+        <v>85</v>
+      </c>
+      <c r="E78" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C79" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>75</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B83" t="s">
         <v>101</v>
       </c>
-      <c r="C80" t="s">
-        <v>84</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="C83" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" t="s">
         <v>85</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E83" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H10" r:id="rId1"/>
-    <hyperlink ref="H31" r:id="rId2"/>
+    <hyperlink ref="H13" r:id="rId1"/>
+    <hyperlink ref="H34" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First go at CruizcoreGyro and claimed DThermalIR
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="152">
   <si>
     <t>AccelHTSensor</t>
   </si>
@@ -466,6 +466,15 @@
   </si>
   <si>
     <t>Should be replaced by an integration filter</t>
+  </si>
+  <si>
+    <t>http://xgl.minfinity.com/Downloads/Downloads.html</t>
+  </si>
+  <si>
+    <t>DexterThermalIR</t>
+  </si>
+  <si>
+    <t>Rate</t>
   </si>
 </sst>
 </file>
@@ -818,13 +827,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I84"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,6 +1090,9 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
       <c r="C15" t="s">
         <v>84</v>
       </c>
@@ -1090,108 +1102,96 @@
       <c r="E15" t="s">
         <v>90</v>
       </c>
+      <c r="F15" t="s">
+        <v>104</v>
+      </c>
       <c r="G15" t="s">
         <v>87</v>
       </c>
+      <c r="H15" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>84</v>
+      <c r="F16" t="s">
+        <v>151</v>
+      </c>
+      <c r="G16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
+      <c r="F17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G17" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" t="s">
-        <v>121</v>
-      </c>
-      <c r="G20" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" t="s">
-        <v>103</v>
-      </c>
-      <c r="E21" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21" t="s">
-        <v>121</v>
-      </c>
-      <c r="G21" t="s">
-        <v>87</v>
-      </c>
-      <c r="H21" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
       </c>
       <c r="C22" t="s">
         <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" t="s">
+        <v>90</v>
+      </c>
+      <c r="F22" t="s">
+        <v>121</v>
+      </c>
+      <c r="G22" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C23" t="s">
         <v>84</v>
@@ -1203,59 +1203,92 @@
         <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G23" t="s">
         <v>87</v>
       </c>
       <c r="H23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B24" t="s">
+        <v>150</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="D24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="C25" t="s">
         <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>90</v>
+      </c>
+      <c r="F25" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
         <v>89</v>
@@ -1263,75 +1296,57 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" t="s">
-        <v>86</v>
-      </c>
-      <c r="G30" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" t="s">
-        <v>87</v>
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>141</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
         <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
       </c>
       <c r="G32" t="s">
         <v>87</v>
       </c>
-      <c r="H32" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-      <c r="I33" t="s">
-        <v>148</v>
+      <c r="F33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>141</v>
       </c>
       <c r="C34" t="s">
         <v>84</v>
@@ -1342,105 +1357,123 @@
       <c r="E34" t="s">
         <v>90</v>
       </c>
-      <c r="F34" t="s">
-        <v>111</v>
-      </c>
       <c r="G34" t="s">
         <v>87</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I34" t="s">
-        <v>93</v>
+      <c r="H34" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
         <v>90</v>
+      </c>
+      <c r="I35" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="B36" t="s">
+        <v>112</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
-      </c>
-      <c r="H36" t="s">
-        <v>94</v>
+        <v>84</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" t="s">
+        <v>90</v>
+      </c>
+      <c r="F36" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" t="s">
+        <v>87</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I36" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" t="s">
-        <v>103</v>
-      </c>
-      <c r="E37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F37" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38" t="s">
-        <v>90</v>
-      </c>
-      <c r="F38" t="s">
-        <v>143</v>
-      </c>
-      <c r="G38" t="s">
-        <v>87</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>145</v>
+        <v>90</v>
+      </c>
+      <c r="H38" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" t="s">
+        <v>103</v>
+      </c>
+      <c r="E39" t="s">
+        <v>90</v>
+      </c>
       <c r="F39" t="s">
         <v>142</v>
       </c>
+      <c r="G39" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" t="s">
+        <v>90</v>
+      </c>
+      <c r="F40" t="s">
+        <v>143</v>
+      </c>
+      <c r="G40" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" t="s">
-        <v>84</v>
+      <c r="F41" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C42" t="s">
         <v>90</v>
@@ -1448,24 +1481,15 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>34</v>
-      </c>
-      <c r="B43" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
         <v>84</v>
-      </c>
-      <c r="D43" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C44" t="s">
         <v>90</v>
@@ -1473,15 +1497,24 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="B45" t="s">
+        <v>102</v>
       </c>
       <c r="C45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C46" t="s">
         <v>90</v>
@@ -1489,7 +1522,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C47" t="s">
         <v>90</v>
@@ -1497,75 +1530,75 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>39</v>
-      </c>
-      <c r="B48" t="s">
-        <v>130</v>
+        <v>37</v>
       </c>
       <c r="C48" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" t="s">
-        <v>90</v>
-      </c>
-      <c r="F48" t="s">
-        <v>129</v>
-      </c>
-      <c r="G48" t="s">
-        <v>87</v>
-      </c>
-      <c r="H48" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>40</v>
-      </c>
-      <c r="B49" t="s">
-        <v>127</v>
+        <v>38</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" t="s">
-        <v>90</v>
-      </c>
-      <c r="F49" t="s">
-        <v>121</v>
-      </c>
-      <c r="G49" t="s">
-        <v>87</v>
-      </c>
-      <c r="H49" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="B50" t="s">
+        <v>130</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="D50" t="s">
+        <v>103</v>
+      </c>
+      <c r="E50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" t="s">
+        <v>87</v>
+      </c>
+      <c r="H50" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B51" t="s">
+        <v>127</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="D51" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" t="s">
+        <v>121</v>
+      </c>
+      <c r="G51" t="s">
+        <v>87</v>
+      </c>
+      <c r="H51" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
         <v>90</v>
@@ -1573,7 +1606,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C53" t="s">
         <v>90</v>
@@ -1581,7 +1614,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C54" t="s">
         <v>90</v>
@@ -1589,18 +1622,15 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
         <v>90</v>
-      </c>
-      <c r="H55" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C56" t="s">
         <v>90</v>
@@ -1608,24 +1638,18 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C57" t="s">
-        <v>84</v>
-      </c>
-      <c r="D57" t="s">
-        <v>103</v>
-      </c>
-      <c r="F57" t="s">
-        <v>131</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>146</v>
+        <v>90</v>
+      </c>
+      <c r="H57" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C58" t="s">
         <v>90</v>
@@ -1633,7 +1657,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
         <v>84</v>
@@ -1642,53 +1666,62 @@
         <v>103</v>
       </c>
       <c r="F59" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C60" t="s">
         <v>90</v>
-      </c>
-      <c r="H60" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
-      </c>
-      <c r="H61" t="s">
-        <v>98</v>
+        <v>84</v>
+      </c>
+      <c r="D61" t="s">
+        <v>103</v>
+      </c>
+      <c r="F61" t="s">
+        <v>122</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C62" t="s">
         <v>90</v>
+      </c>
+      <c r="H62" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C63" t="s">
         <v>90</v>
+      </c>
+      <c r="H63" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C64" t="s">
         <v>90</v>
@@ -1696,30 +1729,15 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
-      </c>
-      <c r="B65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>84</v>
-      </c>
-      <c r="D65" t="s">
-        <v>103</v>
-      </c>
-      <c r="E65" t="s">
-        <v>90</v>
-      </c>
-      <c r="F65" t="s">
-        <v>131</v>
-      </c>
-      <c r="G65" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C66" t="s">
         <v>90</v>
@@ -1727,15 +1745,30 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="B67" t="s">
+        <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="D67" t="s">
+        <v>103</v>
+      </c>
+      <c r="E67" t="s">
+        <v>90</v>
+      </c>
+      <c r="F67" t="s">
+        <v>131</v>
+      </c>
+      <c r="G67" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
         <v>90</v>
@@ -1743,7 +1776,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C69" t="s">
         <v>90</v>
@@ -1751,7 +1784,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C70" t="s">
         <v>90</v>
@@ -1759,15 +1792,15 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C71" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C72" t="s">
         <v>90</v>
@@ -1775,54 +1808,57 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>64</v>
-      </c>
-      <c r="B73" t="s">
-        <v>128</v>
+        <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>84</v>
-      </c>
-      <c r="D73" t="s">
-        <v>103</v>
-      </c>
-      <c r="E73" t="s">
-        <v>90</v>
-      </c>
-      <c r="F73" t="s">
-        <v>125</v>
-      </c>
-      <c r="G73" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C74" t="s">
         <v>90</v>
-      </c>
-      <c r="H74" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="B75" t="s">
+        <v>128</v>
       </c>
       <c r="C75" t="s">
-        <v>90</v>
+        <v>84</v>
+      </c>
+      <c r="D75" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" t="s">
+        <v>90</v>
+      </c>
+      <c r="F75" t="s">
+        <v>125</v>
+      </c>
+      <c r="G75" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="C76" t="s">
+        <v>90</v>
+      </c>
+      <c r="H76" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C77" t="s">
         <v>90</v>
@@ -1830,32 +1866,20 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>69</v>
-      </c>
-      <c r="C78" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>84</v>
-      </c>
-      <c r="D79" t="s">
-        <v>85</v>
-      </c>
-      <c r="E79" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C80" t="s">
         <v>90</v>
@@ -1863,23 +1887,32 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="B81" t="s">
+        <v>101</v>
       </c>
       <c r="C81" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" t="s">
+        <v>85</v>
+      </c>
+      <c r="E81" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C82" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C83" t="s">
         <v>90</v>
@@ -1887,29 +1920,45 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>73</v>
+      </c>
+      <c r="C84" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B86" t="s">
         <v>100</v>
       </c>
-      <c r="C84" t="s">
-        <v>84</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="C86" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86" t="s">
         <v>85</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E86" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H13" r:id="rId1"/>
-    <hyperlink ref="H34" r:id="rId2"/>
+    <hyperlink ref="H36" r:id="rId2"/>
     <hyperlink ref="H9" r:id="rId3"/>
-    <hyperlink ref="H38" r:id="rId4"/>
-    <hyperlink ref="H57" r:id="rId5"/>
-    <hyperlink ref="H59" r:id="rId6"/>
+    <hyperlink ref="H40" r:id="rId4"/>
+    <hyperlink ref="H59" r:id="rId5"/>
+    <hyperlink ref="H61" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor changes to sensor classes
If needed:
1) make them comply to standards: right handed cartesian coordinates,
units
2) Improved normalization
3) setModes added
</commit_message>
<xml_diff>
--- a/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
+++ b/ev3classes/src/lejos/hardware/sensor/Inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
   <si>
     <t>EV3IRSensor</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Needs rework for sampleprovider</t>
   </si>
   <si>
-    <t>Needs testing</t>
-  </si>
-  <si>
     <t>http://www.minfinity.com/Manual/CruizCore_XG1300L_User_Manual.pdf</t>
   </si>
   <si>
@@ -182,16 +179,9 @@
     <t>http://dexterindustries.com/files/dIMU_Datasheets.zip</t>
   </si>
   <si>
-    <t>SensorModes must be implemented</t>
-  </si>
-  <si>
     <t>http://www.dexterindustries.com/Products-dPressure.html</t>
   </si>
   <si>
-    <t>Needs to work with EV3 AD converter
-Replace setTypeAndMode</t>
-  </si>
-  <si>
     <t>http://dexterindustries.com/manual/thermal-infrared-sensor/</t>
   </si>
   <si>
@@ -213,37 +203,16 @@
     <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NBR1036</t>
   </si>
   <si>
-    <t>Does it comply with right hand rule?</t>
-  </si>
-  <si>
     <t>http://www.hitechnic.com/cgi-bin/commerce.cgi?preadd=action&amp;key=NEO1048</t>
   </si>
   <si>
-    <t>Untested</t>
-  </si>
-  <si>
-    <t>Replace setTypeAndMode</t>
-  </si>
-  <si>
     <t>http://www.mindsensors.com/index.php?module=pagemaster&amp;PAGE_user_op=view_page&amp;PAGE_id=101</t>
   </si>
   <si>
-    <t>Inverse Z-axis to comply</t>
-  </si>
-  <si>
     <t>http://www.mindsensors.com/index.php?module=pagemaster&amp;PAGE_user_op=view_page&amp;PAGE_id=56</t>
   </si>
   <si>
     <t>http://www.mindsensors.com/index.php?module=pagemaster&amp;PAGE_user_op=view_page&amp;PAGE_id=168</t>
-  </si>
-  <si>
-    <t>What unit to use? It is Pascal now</t>
-  </si>
-  <si>
-    <t>Use normalize function to normalize</t>
-  </si>
-  <si>
-    <t>Creates new instances of SensorMode on each call</t>
   </si>
   <si>
     <t>Remove calibration 
@@ -253,10 +222,6 @@
     <t>Remove</t>
   </si>
   <si>
-    <t>Replace setTypeAndMode
-Needs to work with EV3 AD converter</t>
-  </si>
-  <si>
     <t>http://www.mindsensors.com/index.php?module=pagemaster&amp;PAGE_user_op=view_page&amp;PAGE_id=75</t>
   </si>
   <si>
@@ -303,13 +268,28 @@
   </si>
   <si>
     <t>Dflex</t>
+  </si>
+  <si>
+    <t>Optional: Use integer mode for higher resolution</t>
+  </si>
+  <si>
+    <t>Changed readFloats in AnalogPort to return normalized values (Check with Andy for possible side effects)</t>
+  </si>
+  <si>
+    <t>Uses setTypeAndMode</t>
+  </si>
+  <si>
+    <t>formula to calculate DPRESS_MULT differed from DexterPressure250. I choose the formula I thought was right but cannot verify this by testing (Aswin)</t>
+  </si>
+  <si>
+    <t>Remark</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +309,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -367,6 +354,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -672,20 +665,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad2"/>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="3" width="42.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -693,386 +686,392 @@
         <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C17" r:id="rId1"/>
-    <hyperlink ref="C27" r:id="rId2"/>
-    <hyperlink ref="C38" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="D17" r:id="rId1"/>
+    <hyperlink ref="D27" r:id="rId2"/>
+    <hyperlink ref="D38" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId4"/>
+    <hyperlink ref="D18" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1080,7 +1079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -1088,10 +1087,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1101,58 +1100,58 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>